<commit_message>
AUT-887 Add eIDAS RequesterID to client form
</commit_message>
<xml_diff>
--- a/tara-admin-api/src/test/resources/import_files/clients.xlsx
+++ b/tara-admin-api/src/test/resources/import_files/clients.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB524F8-245C-449E-8CA2-D40FABD5BEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A16233A-C070-4271-B989-070EF9993030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAS clients" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Institution name</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>^https://tara-client.example.com:8451/oauth/response.*</t>
+  </si>
+  <si>
+    <t>eIDAS RequesterID</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298e</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298a</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298b</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298c</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298d</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298f</t>
+  </si>
+  <si>
+    <t>58ee2267-7864-4e09-958b-b53c3135298g</t>
   </si>
 </sst>
 </file>
@@ -528,31 +552,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="131.5703125" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="131.5546875" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="212.28515625" customWidth="1"/>
-    <col min="14" max="14" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="212.33203125" customWidth="1"/>
+    <col min="14" max="14" width="42.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,10 +617,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -615,8 +642,11 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
+      <c r="N2" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -636,10 +666,13 @@
         <v>16</v>
       </c>
       <c r="N3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -659,10 +692,13 @@
         <v>45</v>
       </c>
       <c r="N4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -681,8 +717,11 @@
       <c r="M5" t="s">
         <v>16</v>
       </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -723,10 +762,13 @@
         <v>40</v>
       </c>
       <c r="N6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -746,10 +788,13 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -769,6 +814,9 @@
         <v>28</v>
       </c>
       <c r="N8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GSSO-588 Add functionality to define allowed IP addresses for clients and an api to request defined IP-s for all clients
</commit_message>
<xml_diff>
--- a/tara-admin-api/src/test/resources/import_files/clients.xlsx
+++ b/tara-admin-api/src/test/resources/import_files/clients.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A16233A-C070-4271-B989-070EF9993030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32DF2D9-A44D-43E0-9527-9F7E41E239A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2940" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAS clients" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Institution name</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>58ee2267-7864-4e09-958b-b53c3135298g</t>
+  </si>
+  <si>
+    <t>Token request allowed IP addresses</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
   </si>
 </sst>
 </file>
@@ -552,31 +558,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="131.5546875" customWidth="1"/>
-    <col min="5" max="5" width="72.33203125" customWidth="1"/>
-    <col min="6" max="6" width="38.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="131.5703125" customWidth="1"/>
+    <col min="5" max="5" width="72.28515625" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="212.33203125" customWidth="1"/>
-    <col min="14" max="14" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="212.28515625" customWidth="1"/>
+    <col min="14" max="14" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +628,11 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -645,8 +654,11 @@
       <c r="N2" t="s">
         <v>50</v>
       </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -671,8 +683,11 @@
       <c r="O3" t="s">
         <v>17</v>
       </c>
+      <c r="P3" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -697,8 +712,11 @@
       <c r="O4" t="s">
         <v>18</v>
       </c>
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -720,8 +738,11 @@
       <c r="N5" t="s">
         <v>53</v>
       </c>
+      <c r="P5" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -767,8 +788,11 @@
       <c r="O6" t="s">
         <v>19</v>
       </c>
+      <c r="P6" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -793,8 +817,11 @@
       <c r="O7" t="s">
         <v>26</v>
       </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -818,6 +845,9 @@
       </c>
       <c r="O8" t="s">
         <v>37</v>
+      </c>
+      <c r="P8" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>